<commit_message>
adding plots, new data
</commit_message>
<xml_diff>
--- a/data/pedagogy_data.xlsx
+++ b/data/pedagogy_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc8e1a904a64e38e/Documents/Oregon/Courses/datascience spec/edld_640/Capstone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc8e1a904a64e38e/Documents/Oregon/Courses/datascience spec/edld_640/EDLD-640-Capstone/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="14_{6BAE1E7B-C09A-4F93-BFB1-1D04A3BB8FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9DE3BF4-D9DF-4461-A1ED-89DE75162D58}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="14_{6BAE1E7B-C09A-4F93-BFB1-1D04A3BB8FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA548DC4-0D8F-4C5F-832B-6604AE988DAB}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="21060" windowHeight="12132" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50130" yWindow="-7755" windowWidth="17280" windowHeight="16965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DD.F22" sheetId="1" r:id="rId1"/>
@@ -1782,7 +1782,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1798,6 +1798,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2015,7 +2021,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -2082,6 +2088,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2428,8 +2436,8 @@
   <dimension ref="A1:J156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J150" sqref="A150:J150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6325,28 +6333,30 @@
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
+      <c r="A150" s="24" t="s">
         <v>477</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="25">
         <v>2</v>
       </c>
-      <c r="E150" s="1">
+      <c r="D150" s="24"/>
+      <c r="E150" s="25">
         <v>8</v>
       </c>
-      <c r="G150" t="s">
+      <c r="F150" s="24"/>
+      <c r="G150" s="24" t="s">
         <v>568</v>
       </c>
-      <c r="H150" t="s">
+      <c r="H150" s="24" t="s">
         <v>476</v>
       </c>
-      <c r="I150" t="s">
+      <c r="I150" s="24" t="s">
         <v>475</v>
       </c>
-      <c r="J150" s="1">
+      <c r="J150" s="25">
         <v>2</v>
       </c>
     </row>

</xml_diff>